<commit_message>
Update file tiến độ
</commit_message>
<xml_diff>
--- a/Document/Tiến độ code các chức năng.xlsx
+++ b/Document/Tiến độ code các chức năng.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Source\ATInnovation\Github\PhamMemChamCong\HeThongChamCong\Document\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
   </bookViews>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="70">
   <si>
     <t>Form</t>
   </si>
@@ -30,9 +35,6 @@
     <t>Tiến độ</t>
   </si>
   <si>
-    <t>Làm</t>
-  </si>
-  <si>
     <t>Máy chấm công</t>
   </si>
   <si>
@@ -165,9 +167,6 @@
     <t>Khai báo trình độ học vấn</t>
   </si>
   <si>
-    <t>Khai báo giới tính</t>
-  </si>
-  <si>
     <t>Kết nối cơ sở dữ liệu</t>
   </si>
   <si>
@@ -223,6 +222,18 @@
   </si>
   <si>
     <t>Cơ sở dữ liệu quan hệ chưa được hoàn thành,  nên chưa viết được stored procedure</t>
+  </si>
+  <si>
+    <t>xong front-end  - Đang làm backend</t>
+  </si>
+  <si>
+    <t>Khai báo server RabbitMQ</t>
+  </si>
+  <si>
+    <t>Yêu cầu mới</t>
+  </si>
+  <si>
+    <t>Thái làm kết nối và lấy ra dữ liệu theo các command status trước khi Sáng làm</t>
   </si>
 </sst>
 </file>
@@ -737,7 +748,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -745,10 +756,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:F47"/>
+  <dimension ref="A2:F51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -758,12 +769,12 @@
     <col min="3" max="3" width="12.5703125" customWidth="1"/>
     <col min="4" max="4" width="15.7109375" customWidth="1"/>
     <col min="5" max="5" width="46.28515625" customWidth="1"/>
-    <col min="6" max="6" width="71.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="75.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:6" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="32" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B2" s="32"/>
       <c r="C2" s="32"/>
@@ -778,187 +789,185 @@
         <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E4" s="17" t="s">
         <v>2</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="22"/>
+      <c r="D5" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="B5" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="C5" s="25" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" s="25" t="s">
-        <v>53</v>
-      </c>
       <c r="E5" s="31" t="s">
-        <v>16</v>
+        <v>58</v>
       </c>
       <c r="F5" s="27"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="24"/>
       <c r="B6" s="25" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C6" s="25"/>
       <c r="D6" s="25" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E6" s="26" t="s">
-        <v>16</v>
+        <v>58</v>
       </c>
       <c r="F6" s="27"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="24"/>
       <c r="B7" s="25" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C7" s="25"/>
       <c r="D7" s="25" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E7" s="26" t="s">
-        <v>16</v>
+        <v>58</v>
       </c>
       <c r="F7" s="27"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="24"/>
       <c r="B8" s="25" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C8" s="25"/>
       <c r="D8" s="25" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E8" s="26" t="s">
-        <v>16</v>
+        <v>56</v>
       </c>
       <c r="F8" s="27"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="24"/>
       <c r="B9" s="25" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C9" s="25"/>
       <c r="D9" s="25" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E9" s="26" t="s">
-        <v>16</v>
+        <v>56</v>
       </c>
       <c r="F9" s="27"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="24"/>
       <c r="B10" s="25" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C10" s="25"/>
       <c r="D10" s="25" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E10" s="26" t="s">
-        <v>16</v>
+        <v>56</v>
       </c>
       <c r="F10" s="27"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="24"/>
       <c r="B11" s="25" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C11" s="25"/>
       <c r="D11" s="25" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E11" s="26" t="s">
-        <v>16</v>
+        <v>56</v>
       </c>
       <c r="F11" s="27"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="24"/>
       <c r="B12" s="25" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C12" s="25"/>
       <c r="D12" s="25" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E12" s="26" t="s">
-        <v>16</v>
+        <v>56</v>
       </c>
       <c r="F12" s="27"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="24"/>
       <c r="B13" s="25" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C13" s="25"/>
       <c r="D13" s="25" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E13" s="26" t="s">
-        <v>16</v>
+        <v>56</v>
       </c>
       <c r="F13" s="27"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="24"/>
       <c r="B14" s="25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C14" s="25"/>
       <c r="D14" s="25" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E14" s="26" t="s">
-        <v>16</v>
+        <v>56</v>
       </c>
       <c r="F14" s="27"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="24"/>
       <c r="B15" s="25" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C15" s="25"/>
       <c r="D15" s="25" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E15" s="26" t="s">
-        <v>16</v>
+        <v>58</v>
       </c>
       <c r="F15" s="27"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="24"/>
       <c r="B16" s="25" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C16" s="25"/>
       <c r="D16" s="25" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E16" s="26" t="s">
-        <v>16</v>
+        <v>58</v>
       </c>
       <c r="F16" s="27"/>
     </row>
@@ -969,173 +978,167 @@
       </c>
       <c r="C17" s="25"/>
       <c r="D17" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="E17" s="26" t="s">
-        <v>16</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="E17" s="26"/>
       <c r="F17" s="27"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="24"/>
-      <c r="B18" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="C18" s="25" t="s">
-        <v>63</v>
-      </c>
-      <c r="D18" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="E18" s="26"/>
+      <c r="A18" s="19"/>
+      <c r="B18" s="23"/>
+      <c r="C18" s="23"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="21"/>
       <c r="F18" s="27"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="19"/>
-      <c r="B19" s="23"/>
-      <c r="C19" s="23"/>
-      <c r="D19" s="23"/>
-      <c r="E19" s="21"/>
-      <c r="F19" s="28"/>
+      <c r="A19" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="B19" s="25"/>
+      <c r="C19" s="25"/>
+      <c r="D19" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E19" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="F19" s="31"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="7" t="s">
+      <c r="A20" s="24"/>
+      <c r="B20" s="25"/>
+      <c r="C20" s="25"/>
+      <c r="D20" s="25"/>
+      <c r="E20" s="26"/>
+      <c r="F20" s="26"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="19"/>
+      <c r="B21" s="23"/>
+      <c r="C21" s="23"/>
+      <c r="D21" s="23"/>
+      <c r="E21" s="21"/>
+      <c r="F21" s="21"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B22" s="14" t="s">
         <v>4</v>
-      </c>
-      <c r="B20" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="C20" s="9"/>
-      <c r="D20" s="26" t="s">
-        <v>56</v>
-      </c>
-      <c r="E20" s="27" t="s">
-        <v>60</v>
-      </c>
-      <c r="F20" s="15"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="7"/>
-      <c r="B21" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C21" s="9"/>
-      <c r="D21" s="26" t="s">
-        <v>56</v>
-      </c>
-      <c r="E21" s="27" t="s">
-        <v>60</v>
-      </c>
-      <c r="F21" s="27"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="7"/>
-      <c r="B22" s="8" t="s">
-        <v>7</v>
       </c>
       <c r="C22" s="9"/>
       <c r="D22" s="26" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E22" s="27" t="s">
-        <v>60</v>
-      </c>
-      <c r="F22" s="27"/>
+        <v>58</v>
+      </c>
+      <c r="F22" s="15"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="7"/>
-      <c r="B23" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C23" s="9"/>
+      <c r="B23" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>68</v>
+      </c>
       <c r="D23" s="26" t="s">
-        <v>56</v>
-      </c>
-      <c r="E23" s="27" t="s">
-        <v>60</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="E23" s="27"/>
       <c r="F23" s="27"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="7"/>
       <c r="B24" s="8" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C24" s="9"/>
       <c r="D24" s="26" t="s">
-        <v>56</v>
-      </c>
-      <c r="E24" s="27"/>
-      <c r="F24" s="27"/>
+        <v>54</v>
+      </c>
+      <c r="E24" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="F24" s="27" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="7"/>
       <c r="B25" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>63</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="C25" s="9"/>
       <c r="D25" s="26" t="s">
-        <v>56</v>
-      </c>
-      <c r="E25" s="27"/>
-      <c r="F25" s="27"/>
+        <v>54</v>
+      </c>
+      <c r="E25" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="F25" s="27" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="7"/>
       <c r="B26" s="8" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C26" s="9"/>
       <c r="D26" s="26" t="s">
-        <v>56</v>
-      </c>
-      <c r="E26" s="27"/>
-      <c r="F26" s="27"/>
+        <v>54</v>
+      </c>
+      <c r="E26" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="F26" s="27" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="10"/>
-      <c r="B27" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C27" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="D27" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="E27" s="27"/>
-      <c r="F27" s="28"/>
+      <c r="A27" s="7"/>
+      <c r="B27" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C27" s="9"/>
+      <c r="D27" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="E27" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="F27" s="27" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B28" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C28" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="D28" s="31" t="s">
-        <v>15</v>
-      </c>
-      <c r="E28" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="F28" s="27" t="s">
-        <v>64</v>
-      </c>
+      <c r="A28" s="7"/>
+      <c r="B28" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="D28" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="E28" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="F28" s="27"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="7"/>
-      <c r="B29" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="C29" s="14"/>
+      <c r="B29" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C29" s="9"/>
       <c r="D29" s="26" t="s">
-        <v>15</v>
+        <v>54</v>
       </c>
       <c r="E29" s="27" t="s">
         <v>58</v>
@@ -1145,266 +1148,324 @@
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="7"/>
       <c r="B30" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="C30" s="14"/>
+        <v>11</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>61</v>
+      </c>
       <c r="D30" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="E30" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="F30" s="27"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="10"/>
+      <c r="B31" s="11"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="21"/>
+      <c r="E31" s="27"/>
+      <c r="F31" s="28"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C32" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="D32" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="E32" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="E30" s="27" t="s">
-        <v>60</v>
-      </c>
-      <c r="F30" s="27" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="7"/>
-      <c r="B31" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="C31" s="14"/>
-      <c r="D31" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="E31" s="27" t="s">
-        <v>60</v>
-      </c>
-      <c r="F31" s="27" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="7"/>
-      <c r="B32" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="C32" s="14"/>
-      <c r="D32" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="E32" s="27" t="s">
-        <v>60</v>
-      </c>
-      <c r="F32" s="27"/>
+      <c r="F32" s="27" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="7"/>
       <c r="B33" s="14" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C33" s="14"/>
       <c r="D33" s="26" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E33" s="27" t="s">
-        <v>60</v>
-      </c>
-      <c r="F33" s="27" t="s">
-        <v>66</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="F33" s="27"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="7"/>
       <c r="B34" s="14" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C34" s="14"/>
       <c r="D34" s="26" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E34" s="27" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F34" s="27" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="10"/>
+      <c r="A35" s="7"/>
       <c r="B35" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C35" s="14"/>
+      <c r="D35" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="E35" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="F35" s="27" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="7"/>
+      <c r="B36" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C36" s="14"/>
+      <c r="D36" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="E36" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="F36" s="27"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="7"/>
+      <c r="B37" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C37" s="14"/>
+      <c r="D37" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="E37" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="F37" s="27" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="7"/>
+      <c r="B38" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C38" s="14"/>
+      <c r="D38" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="E38" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="F38" s="27" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="10"/>
+      <c r="B39" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C39" s="11"/>
+      <c r="D39" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="E39" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="F39" s="27"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="C35" s="11"/>
-      <c r="D35" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="E35" s="28" t="s">
-        <v>60</v>
-      </c>
-      <c r="F35" s="27"/>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="24" t="s">
-        <v>24</v>
-      </c>
-      <c r="B36" s="31"/>
-      <c r="C36" s="9"/>
-      <c r="D36" s="31"/>
-      <c r="E36" s="31"/>
-      <c r="F36" s="31"/>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="24"/>
-      <c r="B37" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="C37" s="9"/>
-      <c r="D37" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="E37" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="F37" s="26"/>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="24"/>
-      <c r="B38" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="C38" s="9"/>
-      <c r="D38" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="E38" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="F38" s="26"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="24"/>
-      <c r="B39" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="C39" s="20" t="s">
-        <v>63</v>
-      </c>
-      <c r="D39" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="E39" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="F39" s="26"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="24"/>
-      <c r="B40" s="14" t="s">
-        <v>29</v>
-      </c>
+      <c r="B40" s="31"/>
       <c r="C40" s="9"/>
-      <c r="D40" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="E40" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="F40" s="26"/>
+      <c r="D40" s="31"/>
+      <c r="E40" s="31"/>
+      <c r="F40" s="31"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="24"/>
       <c r="B41" s="14" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C41" s="9"/>
       <c r="D41" s="26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E41" s="26" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F41" s="26"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="24"/>
       <c r="B42" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="C42" s="9" t="s">
-        <v>63</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="C42" s="9"/>
       <c r="D42" s="26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E42" s="26" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F42" s="26"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="24"/>
       <c r="B43" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C43" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="D43" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="E43" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="F43" s="26"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="24"/>
+      <c r="B44" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C44" s="9"/>
+      <c r="D44" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="E44" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="F44" s="26"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="24"/>
+      <c r="B45" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C45" s="9"/>
+      <c r="D45" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="E45" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="F45" s="26"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="24"/>
+      <c r="B46" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C46" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="D46" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="E46" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="F46" s="26"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="24"/>
+      <c r="B47" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C47" s="9"/>
+      <c r="D47" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="E47" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="F47" s="26"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="19"/>
+      <c r="B48" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="C43" s="9"/>
-      <c r="D43" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="E43" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="F43" s="26"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="19"/>
-      <c r="B44" s="11" t="s">
+      <c r="C48" s="12"/>
+      <c r="D48" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="E48" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="F48" s="26"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C44" s="12"/>
-      <c r="D44" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="E44" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="F44" s="26"/>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="3" t="s">
+      <c r="B49" s="13"/>
+      <c r="C49" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E49" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F49" s="4"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B45" s="13"/>
-      <c r="C45" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D45" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E45" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F45" s="4"/>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="7" t="s">
+      <c r="B50" s="20"/>
+      <c r="C50" s="14"/>
+      <c r="D50" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E50" s="16"/>
+      <c r="F50" s="16" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="B46" s="20"/>
-      <c r="C46" s="14"/>
-      <c r="D46" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="E46" s="16"/>
-      <c r="F46" s="16" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="29" t="s">
+      <c r="B51" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="B47" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="C47" s="30"/>
-      <c r="D47" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E47" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="F47" s="16"/>
+      <c r="C51" s="30"/>
+      <c r="D51" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E51" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="F51" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
ngoc anh update tien do
</commit_message>
<xml_diff>
--- a/Document/Tiến độ code các chức năng.xlsx
+++ b/Document/Tiến độ code các chức năng.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="72">
   <si>
     <t>Form</t>
   </si>
@@ -234,6 +234,12 @@
   </si>
   <si>
     <t>chưa tính công được</t>
+  </si>
+  <si>
+    <t>Xem Hình Chấm Công</t>
+  </si>
+  <si>
+    <t>Cần chú ý vì hình được lưu thẳng vào db dạng binary</t>
   </si>
 </sst>
 </file>
@@ -758,8 +764,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1253,11 +1259,19 @@
       <c r="A36" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="B36" s="31"/>
+      <c r="B36" s="31" t="s">
+        <v>70</v>
+      </c>
       <c r="C36" s="9"/>
-      <c r="D36" s="31"/>
-      <c r="E36" s="31"/>
-      <c r="F36" s="31"/>
+      <c r="D36" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="E36" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="F36" s="31" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="24"/>

</xml_diff>